<commit_message>
Updated for vSphere 6.5 and some other fixes.
</commit_message>
<xml_diff>
--- a/vsphere-configs.xlsx
+++ b/vsphere-configs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new\vmware\Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\operator\Documents\GitHub\vmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -2391,7 +2391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
@@ -5220,7 +5220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -5256,8 +5258,8 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f xml:space="preserve"> "'MyPassword1'"</f>
-        <v>'MyPassword1'</v>
+        <f xml:space="preserve"> "'MyPassword1!'"</f>
+        <v>'MyPassword1!'</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>272</v>

</xml_diff>

<commit_message>
Fixed Thumprint deploy and add new feature. Now you can omit Any - deploy, config, and/or cert replacement.
</commit_message>
<xml_diff>
--- a/vsphere-configs.xlsx
+++ b/vsphere-configs.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="462">
   <si>
     <t>vlan name</t>
   </si>
@@ -1530,6 +1530,12 @@
   </si>
   <si>
     <t>VMware-vCenter-Server-Appliance-6.5.0.5100-4602587_OVF10.ova</t>
+  </si>
+  <si>
+    <t>Config?</t>
+  </si>
+  <si>
+    <t>Certs?</t>
   </si>
 </sst>
 </file>
@@ -2567,617 +2573,654 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z98"/>
+  <dimension ref="A1:AB98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="7.3125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7890625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.05078125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7890625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.89453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.05078125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.05078125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.9453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.20703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="54.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.15625" style="2"/>
-    <col min="26" max="26" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.15625" style="2"/>
+    <col min="2" max="3" width="7.3125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="17.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7890625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.05078125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.26171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7890625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.89453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.05078125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.05078125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.9453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.68359375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.20703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="54.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.15625" style="2"/>
+    <col min="28" max="28" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>457</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="2" t="str">
+      <c r="B2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="str">
         <f xml:space="preserve"> "vcsa-psc1.acme.com"</f>
         <v>vcsa-psc1.acme.com</v>
       </c>
-      <c r="C2" s="2" t="str">
+      <c r="E2" s="2" t="str">
         <f xml:space="preserve"> "vcsa-psc1.acme.com"</f>
         <v>vcsa-psc1.acme.com</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="E2" s="2" t="str">
+      <c r="G2" s="2" t="str">
         <f xml:space="preserve"> "static"</f>
         <v>static</v>
       </c>
-      <c r="F2" s="2" t="str">
+      <c r="H2" s="2" t="str">
         <f xml:space="preserve"> "ipv4"</f>
         <v>ipv4</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <v>24</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="L2" s="2" t="str">
+      <c r="N2" s="2" t="str">
         <f xml:space="preserve"> "True"</f>
         <v>True</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="2" t="str">
+      <c r="Q2" s="2" t="str">
         <f xml:space="preserve"> "ny-esx-1.acme.com"</f>
         <v>ny-esx-1.acme.com</v>
       </c>
-      <c r="P2" s="2" t="str">
+      <c r="R2" s="2" t="str">
         <f xml:space="preserve"> "vcsa-vlan"</f>
         <v>vcsa-vlan</v>
       </c>
-      <c r="Q2" s="2" t="str">
+      <c r="S2" s="2" t="str">
         <f xml:space="preserve"> "Datastore"</f>
         <v>Datastore</v>
       </c>
-      <c r="R2" s="2" t="str">
+      <c r="T2" s="2" t="str">
         <f xml:space="preserve"> "root"</f>
         <v>root</v>
       </c>
-      <c r="S2" s="2" t="str">
+      <c r="U2" s="2" t="str">
         <f xml:space="preserve"> "esxrootpw"</f>
         <v>esxrootpw</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="2" t="str">
+      <c r="W2" s="2" t="str">
         <f xml:space="preserve"> "acme-vm.com"</f>
         <v>acme-vm.com</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B3" s="2" t="str">
+      <c r="B3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="str">
         <f xml:space="preserve"> "vcsa-psc2.acme.com"</f>
         <v>vcsa-psc2.acme.com</v>
       </c>
-      <c r="C3" s="2" t="str">
+      <c r="E3" s="2" t="str">
         <f xml:space="preserve"> "vcsa-psc2.acme.com"</f>
         <v>vcsa-psc2.acme.com</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="E3" s="2" t="str">
+      <c r="G3" s="2" t="str">
         <f xml:space="preserve"> "static"</f>
         <v>static</v>
       </c>
-      <c r="F3" s="2" t="str">
+      <c r="H3" s="2" t="str">
         <f xml:space="preserve"> "ipv4"</f>
         <v>ipv4</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>24</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="L3" s="2" t="str">
+      <c r="N3" s="2" t="str">
         <f xml:space="preserve"> "True"</f>
         <v>True</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="2" t="str">
+      <c r="Q3" s="2" t="str">
         <f xml:space="preserve"> "ca-esx-1.acme.com"</f>
         <v>ca-esx-1.acme.com</v>
       </c>
-      <c r="P3" s="2" t="str">
+      <c r="R3" s="2" t="str">
         <f xml:space="preserve"> "vcsa-vlan"</f>
         <v>vcsa-vlan</v>
       </c>
-      <c r="Q3" s="2" t="str">
+      <c r="S3" s="2" t="str">
         <f xml:space="preserve"> "Datastore"</f>
         <v>Datastore</v>
       </c>
-      <c r="R3" s="2" t="str">
+      <c r="T3" s="2" t="str">
         <f xml:space="preserve"> "root"</f>
         <v>root</v>
       </c>
-      <c r="S3" s="2" t="str">
+      <c r="U3" s="2" t="str">
         <f xml:space="preserve"> "esxrootpw"</f>
         <v>esxrootpw</v>
       </c>
-      <c r="T3" s="2" t="str">
+      <c r="V3" s="2" t="str">
         <f xml:space="preserve"> "vcsa-psc1.acme.com"</f>
         <v>vcsa-psc1.acme.com</v>
       </c>
-      <c r="U3" s="2" t="str">
+      <c r="W3" s="2" t="str">
         <f xml:space="preserve"> "acme-vm.com"</f>
         <v>acme-vm.com</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="E4" s="2" t="str">
+      <c r="G4" s="2" t="str">
         <f xml:space="preserve"> "static"</f>
         <v>static</v>
       </c>
-      <c r="F4" s="2" t="str">
+      <c r="H4" s="2" t="str">
         <f xml:space="preserve"> "ipv4"</f>
         <v>ipv4</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>24</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="L4" s="2" t="str">
+      <c r="N4" s="2" t="str">
         <f xml:space="preserve"> "True"</f>
         <v>True</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="2" t="str">
+      <c r="Q4" s="2" t="str">
         <f xml:space="preserve"> "ny-esx-1.acme.com"</f>
         <v>ny-esx-1.acme.com</v>
       </c>
-      <c r="P4" s="2" t="str">
+      <c r="R4" s="2" t="str">
         <f xml:space="preserve"> "vcsa-vlan"</f>
         <v>vcsa-vlan</v>
       </c>
-      <c r="Q4" s="2" t="str">
+      <c r="S4" s="2" t="str">
         <f xml:space="preserve"> "Datastore"</f>
         <v>Datastore</v>
       </c>
-      <c r="R4" s="2" t="str">
+      <c r="T4" s="2" t="str">
         <f xml:space="preserve"> "root"</f>
         <v>root</v>
       </c>
-      <c r="S4" s="2" t="str">
+      <c r="U4" s="2" t="str">
         <f xml:space="preserve"> "esxrootpw"</f>
         <v>esxrootpw</v>
       </c>
-      <c r="T4" s="2" t="str">
+      <c r="V4" s="2" t="str">
         <f xml:space="preserve"> "vcsa-psc1.acme.com"</f>
         <v>vcsa-psc1.acme.com</v>
       </c>
-      <c r="U4" s="2" t="str">
+      <c r="W4" s="2" t="str">
         <f xml:space="preserve"> "acme-vm.com"</f>
         <v>acme-vm.com</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="AB4" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="E5" s="2" t="str">
+      <c r="G5" s="2" t="str">
         <f xml:space="preserve"> "static"</f>
         <v>static</v>
       </c>
-      <c r="F5" s="2" t="str">
+      <c r="H5" s="2" t="str">
         <f xml:space="preserve"> "ipv4"</f>
         <v>ipv4</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>24</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="L5" s="2" t="str">
+      <c r="N5" s="2" t="str">
         <f xml:space="preserve"> "True"</f>
         <v>True</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="O5" s="2" t="str">
+      <c r="Q5" s="2" t="str">
         <f xml:space="preserve"> "ca-esx-1.acme.com"</f>
         <v>ca-esx-1.acme.com</v>
       </c>
-      <c r="P5" s="2" t="str">
+      <c r="R5" s="2" t="str">
         <f xml:space="preserve"> "vcsa-vlan"</f>
         <v>vcsa-vlan</v>
       </c>
-      <c r="Q5" s="2" t="str">
+      <c r="S5" s="2" t="str">
         <f xml:space="preserve"> "Datastore"</f>
         <v>Datastore</v>
       </c>
-      <c r="R5" s="2" t="str">
+      <c r="T5" s="2" t="str">
         <f xml:space="preserve"> "root"</f>
         <v>root</v>
       </c>
-      <c r="S5" s="2" t="str">
+      <c r="U5" s="2" t="str">
         <f xml:space="preserve"> "esxrootpw"</f>
         <v>esxrootpw</v>
       </c>
-      <c r="T5" s="2" t="str">
+      <c r="V5" s="2" t="str">
         <f xml:space="preserve"> "vcsa-psc2.acme.com"</f>
         <v>vcsa-psc2.acme.com</v>
       </c>
-      <c r="U5" s="2" t="str">
+      <c r="W5" s="2" t="str">
         <f xml:space="preserve"> "acme-vm.com"</f>
         <v>acme-vm.com</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="Y5" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="Z5" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z6" s="2" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB6" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z7" s="2" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB7" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z8" s="2" t="s">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB8" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z9" s="2" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB9" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="8"/>
-      <c r="Z10" s="2" t="s">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10" s="8"/>
+      <c r="AB10" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z11" s="2" t="s">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB11" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z12" s="2" t="s">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB12" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z13" s="2" t="s">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB13" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z14" s="2" t="s">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB14" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z15" s="4" t="s">
+    <row r="15" spans="1:28" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB15" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z16" s="2" t="s">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB16" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z17" s="2" t="s">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB17" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z18" s="2" t="s">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB18" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z19" s="2" t="s">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB19" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="4"/>
-      <c r="Z20" s="2" t="s">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="4"/>
+      <c r="AB20" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z21" s="2" t="s">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB21" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z22" s="2" t="s">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB22" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z23" s="2" t="s">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB23" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="Z24" s="2" t="s">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB24" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="8"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C43" s="4"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" s="8"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D33" s="8"/>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E43" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" s="8"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B56" s="8"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C66" s="4"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B75" s="8"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56" s="8"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E66" s="4"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B77" s="8"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B78" s="8"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B79" s="8"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C89" s="4"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B98" s="8"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D79" s="8"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E89" s="4"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D98" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>